<commit_message>
Add "Obs" fields for all variables
</commit_message>
<xml_diff>
--- a/reports/COMPADRE_Kendall_protocol.xlsx
+++ b/reports/COMPADRE_Kendall_protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendall/Box Sync/Home/MPM-errors/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C589FE32-EBD8-9D4F-A159-2D1EB439FA23}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CC7365DF-5EEB-D548-9726-110F1AE22BA5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>CompadrinoName</t>
   </si>
@@ -120,12 +120,6 @@
     <t>MeanStageFirstRep</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
-    <t>Long</t>
-  </si>
-  <si>
     <t>MeanStageDuration</t>
   </si>
   <si>
@@ -154,6 +148,39 @@
   </si>
   <si>
     <t>Caswell6.103</t>
+  </si>
+  <si>
+    <t>CensusTypeObs</t>
+  </si>
+  <si>
+    <t>SurvInRepObs</t>
+  </si>
+  <si>
+    <t>MeanAgeFirstRepObs</t>
+  </si>
+  <si>
+    <t>MeanStageFirstRepObs</t>
+  </si>
+  <si>
+    <t>MeanStageDurationObs</t>
+  </si>
+  <si>
+    <t>VarStateDurationObs</t>
+  </si>
+  <si>
+    <t>GrowthTransitionObs</t>
+  </si>
+  <si>
+    <t>LongStages</t>
+  </si>
+  <si>
+    <t>LongStagesObs</t>
+  </si>
+  <si>
+    <t>ReproWithMaturation</t>
+  </si>
+  <si>
+    <t>ReproWithMaturationObs</t>
   </si>
 </sst>
 </file>
@@ -514,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC16C70-3AD3-0840-9DA4-3FC542326147}">
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,19 +560,28 @@
     <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,117 +619,144 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>35</v>
+      <c r="AE1" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="J2" t="s">
         <v>12</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>12</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>23</v>
       </c>
-      <c r="V2" t="s">
-        <v>36</v>
+      <c r="AD2" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="J3" t="s">
         <v>13</v>
       </c>
       <c r="L3" t="s">
         <v>15</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>13</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>24</v>
       </c>
-      <c r="V3" t="s">
-        <v>37</v>
+      <c r="AD3" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="L4" t="s">
         <v>16</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>21</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>25</v>
       </c>
-      <c r="V4" t="s">
-        <v>42</v>
+      <c r="AD4" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="L5" t="s">
         <v>17</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>26</v>
       </c>
-      <c r="V5" t="s">
-        <v>38</v>
+      <c r="AD5" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="L6" t="s">
         <v>18</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>27</v>
       </c>
-      <c r="V6" t="s">
+      <c r="AD6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="P7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AD8" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="O7" t="s">
-        <v>28</v>
-      </c>
-      <c r="V7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="V8" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "Other" to GrowthTransition options
</commit_message>
<xml_diff>
--- a/reports/COMPADRE_Kendall_protocol.xlsx
+++ b/reports/COMPADRE_Kendall_protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendall/Box Sync/Home/MPM-errors/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{621FDA98-1D3A-4B46-A1D8-010378424065}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0FC3EFF9-4590-664F-A45D-D41F6908AB85}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
+    <workbookView xWindow="19600" yWindow="4900" windowWidth="28040" windowHeight="17440" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>CompadrinoName</t>
   </si>
@@ -117,9 +117,6 @@
     <t>MeanAgeFirstRep</t>
   </si>
   <si>
-    <t>MeanStageFirstRep</t>
-  </si>
-  <si>
     <t>MeanStageDuration</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>MeanAgeFirstRepObs</t>
   </si>
   <si>
-    <t>MeanStageFirstRepObs</t>
-  </si>
-  <si>
     <t>MeanStageDurationObs</t>
   </si>
   <si>
@@ -184,6 +178,15 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>StageFirstRep</t>
+  </si>
+  <si>
+    <t>StageFirstRepObs</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -544,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC16C70-3AD3-0840-9DA4-3FC542326147}">
-  <dimension ref="A1:AE9"/>
+  <dimension ref="A1:AE10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,7 +625,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>19</v>
@@ -634,49 +637,49 @@
         <v>22</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
@@ -693,7 +696,7 @@
         <v>23</v>
       </c>
       <c r="AD2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
@@ -710,7 +713,7 @@
         <v>24</v>
       </c>
       <c r="AD3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -724,7 +727,7 @@
         <v>25</v>
       </c>
       <c r="AD4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
@@ -735,7 +738,7 @@
         <v>26</v>
       </c>
       <c r="AD5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
@@ -746,31 +749,36 @@
         <v>27</v>
       </c>
       <c r="AD6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="L7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P7" t="s">
         <v>28</v>
       </c>
       <c r="AD7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="P8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AD8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="AD9" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AD10" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revision to Reproductive Maturity section in response to Rob's comments.
</commit_message>
<xml_diff>
--- a/reports/COMPADRE_Kendall_protocol.xlsx
+++ b/reports/COMPADRE_Kendall_protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendall/Box Sync/Home/MPM-errors/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0FC3EFF9-4590-664F-A45D-D41F6908AB85}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FDC09C12-C58D-434A-B15D-BC3FEF282189}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19600" yWindow="4900" windowWidth="28040" windowHeight="17440" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>CompadrinoName</t>
   </si>
@@ -84,15 +84,6 @@
     <t>Flow</t>
   </si>
   <si>
-    <t>AmbiguousAgeRange</t>
-  </si>
-  <si>
-    <t>AmbiguousAgeRangeObs</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>SurvInRep</t>
   </si>
   <si>
@@ -187,6 +178,9 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>Ambiguous</t>
   </si>
 </sst>
 </file>
@@ -547,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC16C70-3AD3-0840-9DA4-3FC542326147}">
-  <dimension ref="A1:AE10"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AD11" sqref="AD11"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,27 +561,25 @@
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -625,64 +617,58 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="J2" t="s">
         <v>12</v>
       </c>
@@ -690,16 +676,16 @@
         <v>14</v>
       </c>
       <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" t="s">
         <v>12</v>
       </c>
-      <c r="P2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AB2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="J3" t="s">
         <v>13</v>
       </c>
@@ -707,78 +693,81 @@
         <v>15</v>
       </c>
       <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" t="s">
         <v>13</v>
       </c>
-      <c r="P3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AB3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L4" t="s">
         <v>16</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="T4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L5" t="s">
         <v>17</v>
       </c>
-      <c r="P5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="N5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L6" t="s">
         <v>18</v>
       </c>
-      <c r="P6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="N6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="L8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AB9" t="s">
         <v>50</v>
       </c>
-      <c r="P7" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="P8" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="AD9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="AD10" t="s">
-        <v>50</v>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AB10" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add fields for corrected citation information
</commit_message>
<xml_diff>
--- a/reports/COMPADRE_Kendall_protocol.xlsx
+++ b/reports/COMPADRE_Kendall_protocol.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendall/Box Sync/Home/MPM-errors/reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bkendall/Documents/github-bitbucket/MPM-errors/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FDC09C12-C58D-434A-B15D-BC3FEF282189}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F4737AD9-EF99-E54D-B31A-164570A410EA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19600" yWindow="4900" windowWidth="28040" windowHeight="17440" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>CompadrinoName</t>
   </si>
@@ -33,12 +33,6 @@
     <t>ValidatedBy</t>
   </si>
   <si>
-    <t>DOI</t>
-  </si>
-  <si>
-    <t>SpeciesAuthor</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
@@ -181,6 +175,18 @@
   </si>
   <si>
     <t>Ambiguous</t>
+  </si>
+  <si>
+    <t>Author.corr</t>
+  </si>
+  <si>
+    <t>Journal.corr</t>
+  </si>
+  <si>
+    <t>YearPublication.corr</t>
+  </si>
+  <si>
+    <t>DOI.ISBN.corr</t>
   </si>
 </sst>
 </file>
@@ -541,45 +547,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC16C70-3AD3-0840-9DA4-3FC542326147}">
-  <dimension ref="A1:AC10"/>
+  <dimension ref="A1:AE10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="15.83203125" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,46 +607,46 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="T1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>43</v>
@@ -650,124 +655,130 @@
         <v>44</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD2" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD3" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" t="s">
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
         <v>14</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P4" t="s">
         <v>20</v>
       </c>
-      <c r="T2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB2" t="s">
+      <c r="V4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="N5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB3" t="s">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="N6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" t="s">
-        <v>22</v>
-      </c>
-      <c r="T4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" t="s">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="N7" t="s">
+        <v>49</v>
+      </c>
+      <c r="P7" t="s">
         <v>23</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AD7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L6" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB6" t="s">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="N8" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L7" t="s">
-        <v>51</v>
-      </c>
-      <c r="N7" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N8" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="AB9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="AB10" t="s">
-        <v>47</v>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AD9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AD10" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add fields (and instructions) for specifying a model within a study
</commit_message>
<xml_diff>
--- a/reports/COMPADRE_Kendall_protocol.xlsx
+++ b/reports/COMPADRE_Kendall_protocol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bkendall/Documents/github-bitbucket/MPM-errors/reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendall/Documents/Github/MPM-errors/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F4737AD9-EF99-E54D-B31A-164570A410EA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C5A2BDEA-D9FC-C94F-A056-2A42007950F9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19600" yWindow="4900" windowWidth="28040" windowHeight="17440" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
+    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
   <si>
     <t>CompadrinoName</t>
   </si>
@@ -187,6 +187,45 @@
   </si>
   <si>
     <t>DOI.ISBN.corr</t>
+  </si>
+  <si>
+    <t>MatrixIDfield</t>
+  </si>
+  <si>
+    <t>MatrixIDvalue</t>
+  </si>
+  <si>
+    <t>MatrixIDfield2</t>
+  </si>
+  <si>
+    <t>MatrixIDvalue2</t>
+  </si>
+  <si>
+    <t>SpeciesAuthor</t>
+  </si>
+  <si>
+    <t>MatrixPopulation</t>
+  </si>
+  <si>
+    <t>MatrixTreatment</t>
+  </si>
+  <si>
+    <t>MatrixStartYear</t>
+  </si>
+  <si>
+    <t>MatrixStartSeason</t>
+  </si>
+  <si>
+    <t>MatrixStartMonth</t>
+  </si>
+  <si>
+    <t>MatrixEndYear</t>
+  </si>
+  <si>
+    <t>MatrixEndSeason</t>
+  </si>
+  <si>
+    <t>MatrixEndMonth</t>
   </si>
 </sst>
 </file>
@@ -547,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC16C70-3AD3-0840-9DA4-3FC542326147}">
-  <dimension ref="A1:AE10"/>
+  <dimension ref="A1:AI10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,26 +604,27 @@
     <col min="8" max="11" width="15.83203125" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="17.33203125" customWidth="1"/>
+    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -625,159 +665,225 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="L2" t="s">
         <v>10</v>
       </c>
       <c r="N2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P2" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" t="s">
         <v>12</v>
       </c>
-      <c r="P2" t="s">
+      <c r="T2" t="s">
         <v>18</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Z2" t="s">
         <v>10</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AH2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="L3" t="s">
         <v>11</v>
       </c>
       <c r="N3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" t="s">
         <v>13</v>
       </c>
-      <c r="P3" t="s">
+      <c r="T3" t="s">
         <v>19</v>
       </c>
-      <c r="V3" t="s">
+      <c r="Z3" t="s">
         <v>11</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AH3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="N4" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" t="s">
         <v>14</v>
       </c>
-      <c r="P4" t="s">
+      <c r="T4" t="s">
         <v>20</v>
       </c>
-      <c r="V4" t="s">
+      <c r="Z4" t="s">
         <v>45</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AH4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="N5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R5" t="s">
         <v>15</v>
       </c>
-      <c r="P5" t="s">
+      <c r="T5" t="s">
         <v>21</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AH5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="N6" t="s">
+        <v>62</v>
+      </c>
+      <c r="P6" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" t="s">
         <v>16</v>
       </c>
-      <c r="P6" t="s">
+      <c r="T6" t="s">
         <v>22</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AH6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="N7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R7" t="s">
         <v>49</v>
       </c>
-      <c r="P7" t="s">
+      <c r="T7" t="s">
         <v>23</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AH7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="N8" t="s">
+        <v>64</v>
+      </c>
+      <c r="P8" t="s">
+        <v>64</v>
+      </c>
+      <c r="R8" t="s">
         <v>45</v>
       </c>
-      <c r="P8" t="s">
+      <c r="T8" t="s">
         <v>45</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AH8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="AD9" t="s">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="N9" t="s">
+        <v>65</v>
+      </c>
+      <c r="P9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="AD10" t="s">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="N10" t="s">
+        <v>66</v>
+      </c>
+      <c r="P10" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH10" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add a notes field for source corrections
</commit_message>
<xml_diff>
--- a/reports/COMPADRE_Kendall_protocol.xlsx
+++ b/reports/COMPADRE_Kendall_protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendall/Documents/Github/MPM-errors/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C5A2BDEA-D9FC-C94F-A056-2A42007950F9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C48BE5AD-736F-634A-BDEF-3DD6704C60D8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
   <si>
     <t>CompadrinoName</t>
   </si>
@@ -33,9 +33,6 @@
     <t>ValidatedBy</t>
   </si>
   <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>Journal</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>DOI.ISBN</t>
   </si>
   <si>
-    <t>AdditionalSources</t>
-  </si>
-  <si>
     <t>MatrixModified</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>Ambiguous</t>
   </si>
   <si>
-    <t>Author.corr</t>
-  </si>
-  <si>
     <t>Journal.corr</t>
   </si>
   <si>
@@ -226,6 +217,18 @@
   </si>
   <si>
     <t>MatrixEndMonth</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>AdditionalSource</t>
+  </si>
+  <si>
+    <t>Authors.corr</t>
+  </si>
+  <si>
+    <t>SourceCorrectionObs</t>
   </si>
 </sst>
 </file>
@@ -586,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC16C70-3AD3-0840-9DA4-3FC542326147}">
-  <dimension ref="A1:AI10"/>
+  <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,30 +604,30 @@
     <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="15.83203125" customWidth="1"/>
-    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="17.33203125" customWidth="1"/>
-    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="15.83203125" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="17.33203125" customWidth="1"/>
+    <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,259 +635,262 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="O3" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q3" t="s">
+        <v>56</v>
+      </c>
+      <c r="S3" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="O4" t="s">
         <v>57</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="Q4" t="s">
+        <v>57</v>
+      </c>
+      <c r="S4" t="s">
+        <v>12</v>
+      </c>
+      <c r="U4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="O5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>58</v>
+      </c>
+      <c r="S5" t="s">
+        <v>13</v>
+      </c>
+      <c r="U5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="O6" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>59</v>
+      </c>
+      <c r="S6" t="s">
+        <v>14</v>
+      </c>
+      <c r="U6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="O7" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>60</v>
+      </c>
+      <c r="S7" t="s">
+        <v>47</v>
+      </c>
+      <c r="U7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="O8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>61</v>
+      </c>
+      <c r="S8" t="s">
+        <v>43</v>
+      </c>
+      <c r="U8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="O9" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI9" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="O10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI10" t="s">
         <v>43</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="L2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" t="s">
-        <v>58</v>
-      </c>
-      <c r="P2" t="s">
-        <v>58</v>
-      </c>
-      <c r="R2" t="s">
-        <v>12</v>
-      </c>
-      <c r="T2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="L3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P3" t="s">
-        <v>59</v>
-      </c>
-      <c r="R3" t="s">
-        <v>13</v>
-      </c>
-      <c r="T3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="N4" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" t="s">
-        <v>60</v>
-      </c>
-      <c r="R4" t="s">
-        <v>14</v>
-      </c>
-      <c r="T4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="N5" t="s">
-        <v>61</v>
-      </c>
-      <c r="P5" t="s">
-        <v>61</v>
-      </c>
-      <c r="R5" t="s">
-        <v>15</v>
-      </c>
-      <c r="T5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="N6" t="s">
-        <v>62</v>
-      </c>
-      <c r="P6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R6" t="s">
-        <v>16</v>
-      </c>
-      <c r="T6" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="N7" t="s">
-        <v>63</v>
-      </c>
-      <c r="P7" t="s">
-        <v>63</v>
-      </c>
-      <c r="R7" t="s">
-        <v>49</v>
-      </c>
-      <c r="T7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="N8" t="s">
-        <v>64</v>
-      </c>
-      <c r="P8" t="s">
-        <v>64</v>
-      </c>
-      <c r="R8" t="s">
-        <v>45</v>
-      </c>
-      <c r="T8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="N9" t="s">
-        <v>65</v>
-      </c>
-      <c r="P9" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="N10" t="s">
-        <v>66</v>
-      </c>
-      <c r="P10" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "Observation" as a field for IDing matrix
</commit_message>
<xml_diff>
--- a/reports/COMPADRE_Kendall_protocol.xlsx
+++ b/reports/COMPADRE_Kendall_protocol.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendall/Documents/Github/MPM-errors/reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bkendall/Documents/github-bitbucket/MPM-errors/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C48BE5AD-736F-634A-BDEF-3DD6704C60D8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{27F1B72F-6D7E-0A41-9C6E-05EAF434A35E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>CompadrinoName</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>SourceCorrectionObs</t>
+  </si>
+  <si>
+    <t>Observation</t>
   </si>
 </sst>
 </file>
@@ -589,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC16C70-3AD3-0840-9DA4-3FC542326147}">
-  <dimension ref="A1:AJ10"/>
+  <dimension ref="A1:AJ11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L1:L1048576"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -893,6 +896,14 @@
         <v>43</v>
       </c>
     </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="O11" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Fix header for ClassFirstRep
</commit_message>
<xml_diff>
--- a/reports/COMPADRE_Kendall_protocol.xlsx
+++ b/reports/COMPADRE_Kendall_protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendall/Documents/Github/MPM-errors/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FE8986D5-4FCA-B545-9D04-0813F26652CE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{94677ABD-3D45-8C48-9D34-043693DD4E25}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
   </bookViews>
@@ -159,12 +159,6 @@
     <t>Unknown</t>
   </si>
   <si>
-    <t>StageFirstRep</t>
-  </si>
-  <si>
-    <t>StageFirstRepObs</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
@@ -235,6 +229,12 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>ClassFirstRep</t>
+  </si>
+  <si>
+    <t>ClassFirstRepObs</t>
   </si>
 </sst>
 </file>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC16C70-3AD3-0840-9DA4-3FC542326147}">
   <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -653,22 +653,22 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>5</v>
@@ -677,16 +677,16 @@
         <v>7</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>6</v>
@@ -707,10 +707,10 @@
         <v>35</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>41</v>
@@ -748,10 +748,10 @@
         <v>8</v>
       </c>
       <c r="O2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S2" t="s">
         <v>10</v>
@@ -771,10 +771,10 @@
         <v>9</v>
       </c>
       <c r="O3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Q3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="S3" t="s">
         <v>11</v>
@@ -791,13 +791,13 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="M4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Q4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S4" t="s">
         <v>12</v>
@@ -814,10 +814,10 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="O5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S5" t="s">
         <v>13</v>
@@ -831,10 +831,10 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="O6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Q6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S6" t="s">
         <v>14</v>
@@ -848,13 +848,13 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="O7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="S7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U7" t="s">
         <v>21</v>
@@ -865,10 +865,10 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="O8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Q8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S8" t="s">
         <v>43</v>
@@ -882,21 +882,21 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="O9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AI9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="O10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AI10" t="s">
         <v>43</v>
@@ -904,10 +904,10 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="O11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change NA to No Matrix in MatrixModified
</commit_message>
<xml_diff>
--- a/reports/COMPADRE_Kendall_protocol.xlsx
+++ b/reports/COMPADRE_Kendall_protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendall/Documents/Github/MPM-errors/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{94677ABD-3D45-8C48-9D34-043693DD4E25}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C98C113C-7DC4-4446-920C-1D9775C4D0DF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
   </bookViews>
@@ -228,13 +228,13 @@
     <t>Observation</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>ClassFirstRep</t>
   </si>
   <si>
     <t>ClassFirstRepObs</t>
+  </si>
+  <si>
+    <t>No Matrix</t>
   </si>
 </sst>
 </file>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC16C70-3AD3-0840-9DA4-3FC542326147}">
   <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,10 +707,10 @@
         <v>35</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>41</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="M4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O4" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Added drop-down lists for the fields with fixed responses
</commit_message>
<xml_diff>
--- a/reports/COMPADRE_Kendall_protocol.xlsx
+++ b/reports/COMPADRE_Kendall_protocol.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendall/Documents/Github/MPM-errors/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C98C113C-7DC4-4446-920C-1D9775C4D0DF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{35471F75-E098-E14D-A9F2-D90D2E41E038}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
+    <workbookView xWindow="760" yWindow="560" windowWidth="27540" windowHeight="28240" activeTab="1" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data entry" sheetId="1" r:id="rId1"/>
+    <sheet name="Data validation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
   <si>
     <t>CompadrinoName</t>
   </si>
@@ -285,7 +286,116 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -296,6 +406,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{433EE0A3-4B87-0247-A3BF-1D1DB14A708E}" name="Table1" displayName="Table1" ref="A1:A4" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:A4" xr:uid="{8DF710E5-F45F-954B-994D-A54397A5CBF6}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{E0F641A9-2F1A-8D40-87BC-09E2A3AEE8D6}" name="MatrixModified"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{426EB95F-5B5F-C146-A348-6EB236FD555C}" name="Table2" displayName="Table2" ref="C1:C11" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="C1:C11" xr:uid="{0FD91723-BBA2-3D48-A4EF-A9FC42395DDE}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{36BC3137-E852-E749-89DA-980FBFD4BCF2}" name="MatrixIDfield"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{025A96BD-AF3E-3549-A32E-BD5972560322}" name="Table4" displayName="Table4" ref="E1:E8" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="E1:E8" xr:uid="{7B113894-77EE-964E-9CE6-F4C12F3D5592}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{A9223241-E40E-A14D-810C-8F8E3D2B52F2}" name="CensusType"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7763F87B-1AC7-684E-AA9C-BAC87BB06EFB}" name="Table5" displayName="Table5" ref="G1:G8" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="G1:G8" xr:uid="{60043543-DFA1-5341-AB80-A14D18687A8F}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{E747D06A-67FA-0544-B957-762E14AC16F0}" name="SurvInRep"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A694995D-73E0-C248-9B0D-58D4B82CE25A}" name="Table6" displayName="Table6" ref="I1:I4" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="I1:I4" xr:uid="{6FCEC43C-0473-FD4B-BB8F-DAE884ACB031}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{064957DE-CC33-6A4E-9300-B14D983CC94B}" name="ReproWithMaturation"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B4F27360-D890-C948-8746-9588755AF811}" name="Table7" displayName="Table7" ref="K1:K10" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="K1:K10" xr:uid="{30D52A6F-B70F-084F-B3CD-D76D30BE3B18}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{36549443-ED21-1249-8BDF-DDB21DF9FBAC}" name="GrowthTransition"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -595,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC16C70-3AD3-0840-9DA4-3FC542326147}">
-  <dimension ref="A1:AJ11"/>
+  <dimension ref="A1:AJ1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AJ9" sqref="AJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,175 +913,248 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="M2" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E5D4C4E3-0B37-E346-A2D8-D29FA6189E0C}">
+          <x14:formula1>
+            <xm:f>'Data validation'!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>M2:M201</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D013106D-C7E7-CA4C-BA12-73D513A53D1C}">
+          <x14:formula1>
+            <xm:f>'Data validation'!$C$2:$C$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2:O201 Q2:Q201</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9A868832-04AB-BE4D-BD48-11FD0A766C80}">
+          <x14:formula1>
+            <xm:f>'Data validation'!$E$2:$E$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>S2:S201</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{812D6A6A-6C73-B945-A2D7-7CA2FD6A5214}">
+          <x14:formula1>
+            <xm:f>'Data validation'!$G$2:$G$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>U2:U201</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ACC5EE50-0C48-2F47-A792-0FFA3794EB3D}">
+          <x14:formula1>
+            <xm:f>'Data validation'!$I$2:$I$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>AA2:AA201</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4F563273-2072-E746-807E-CF9BF424E291}">
+          <x14:formula1>
+            <xm:f>'Data validation'!$K$2:$K$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>AI2:AI201</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7566CDC-26F2-5142-958C-480AEE553563}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="O2" t="s">
+      <c r="C2" t="s">
         <v>53</v>
       </c>
-      <c r="Q2" t="s">
-        <v>53</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="U2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="K2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="M3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="O3" t="s">
+      <c r="C3" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" t="s">
-        <v>54</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="U3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="I3" t="s">
         <v>9</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="K3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="M4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>69</v>
       </c>
-      <c r="O4" t="s">
+      <c r="C4" t="s">
         <v>55</v>
       </c>
-      <c r="Q4" t="s">
-        <v>55</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="U4" t="s">
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="I4" t="s">
         <v>43</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="K4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="O5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
         <v>56</v>
       </c>
-      <c r="Q5" t="s">
-        <v>56</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="U5" t="s">
+      <c r="G5" t="s">
         <v>19</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="K5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="O6" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="Q6" t="s">
-        <v>57</v>
-      </c>
-      <c r="S6" t="s">
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="U6" t="s">
+      <c r="G6" t="s">
         <v>20</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="K6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="O7" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" t="s">
-        <v>58</v>
-      </c>
-      <c r="S7" t="s">
+      <c r="E7" t="s">
         <v>45</v>
       </c>
-      <c r="U7" t="s">
+      <c r="G7" t="s">
         <v>21</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="K7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="O8" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
         <v>59</v>
       </c>
-      <c r="Q8" t="s">
-        <v>59</v>
-      </c>
-      <c r="S8" t="s">
+      <c r="E8" t="s">
         <v>43</v>
       </c>
-      <c r="U8" t="s">
+      <c r="G8" t="s">
         <v>43</v>
       </c>
-      <c r="AI8" t="s">
+      <c r="K8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="O9" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
         <v>60</v>
       </c>
-      <c r="Q9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI9" t="s">
+      <c r="K9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="O10" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
         <v>61</v>
       </c>
-      <c r="Q10" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI10" t="s">
+      <c r="K10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="O11" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q11" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="6">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added date fields to blank evaluation spreadsheet
</commit_message>
<xml_diff>
--- a/reports/COMPADRE_Kendall_protocol.xlsx
+++ b/reports/COMPADRE_Kendall_protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10610"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendall/Documents/Github/MPM-errors/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B446FFDF-114A-A548-BF7A-B190D61F55F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{39276F0F-9FB9-4741-BA06-B033127D49FD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="560" windowWidth="27540" windowHeight="28240" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="27540" windowHeight="17540" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data entry" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>CompadrinoName</t>
   </si>
@@ -236,6 +236,12 @@
   </si>
   <si>
     <t>No Matrix</t>
+  </si>
+  <si>
+    <t>EntryDate</t>
+  </si>
+  <si>
+    <t>ValidationDate</t>
   </si>
 </sst>
 </file>
@@ -765,151 +771,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC16C70-3AD3-0840-9DA4-3FC542326147}">
-  <dimension ref="A1:AJ1"/>
+  <dimension ref="A1:AL1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="15.83203125" customWidth="1"/>
-    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="17.33203125" customWidth="1"/>
-    <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="15.83203125" customWidth="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="17.33203125" customWidth="1"/>
+    <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.5" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -923,37 +937,37 @@
           <x14:formula1>
             <xm:f>'Data validation'!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M201</xm:sqref>
+          <xm:sqref>O2:O201</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D013106D-C7E7-CA4C-BA12-73D513A53D1C}">
           <x14:formula1>
             <xm:f>'Data validation'!$C$2:$C$11</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O201 Q2:Q201</xm:sqref>
+          <xm:sqref>Q2:Q201 S2:S201</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9A868832-04AB-BE4D-BD48-11FD0A766C80}">
           <x14:formula1>
             <xm:f>'Data validation'!$E$2:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>S2:S201</xm:sqref>
+          <xm:sqref>U2:U201</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{812D6A6A-6C73-B945-A2D7-7CA2FD6A5214}">
           <x14:formula1>
             <xm:f>'Data validation'!$G$2:$G$8</xm:f>
           </x14:formula1>
-          <xm:sqref>U2:U201</xm:sqref>
+          <xm:sqref>W2:W201</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ACC5EE50-0C48-2F47-A792-0FFA3794EB3D}">
           <x14:formula1>
             <xm:f>'Data validation'!$I$2:$I$4</xm:f>
           </x14:formula1>
-          <xm:sqref>AA2:AA201</xm:sqref>
+          <xm:sqref>AC2:AC201</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4F563273-2072-E746-807E-CF9BF424E291}">
           <x14:formula1>
             <xm:f>'Data validation'!$K$2:$K$10</xm:f>
           </x14:formula1>
-          <xm:sqref>AI2:AI201</xm:sqref>
+          <xm:sqref>AK2:AK201</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>